<commit_message>
Speaker to recording dialog, just to save
</commit_message>
<xml_diff>
--- a/formats/excel/one_recipe.xlsx
+++ b/formats/excel/one_recipe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="WhiteSmallBread" sheetId="4" r:id="rId4"/>
     <sheet name="SupersoftSourdoughDohnut" sheetId="5" r:id="rId5"/>
     <sheet name="TartineBrioche" sheetId="6" r:id="rId6"/>
+    <sheet name="Borodinsky-2" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="131">
   <si>
     <t>amount</t>
   </si>
@@ -263,9 +265,6 @@
     <t>sugar for coating</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -326,17 +325,107 @@
     <t>Scalling 1/3</t>
   </si>
   <si>
-    <t>Unsalted butten</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>recipe name</t>
+  </si>
+  <si>
+    <t>Tartine Brioche</t>
+  </si>
+  <si>
+    <t>Unsalted butter</t>
+  </si>
+  <si>
+    <t>wholemeal (dark) rye flour</t>
+  </si>
+  <si>
+    <t>very warm water (at 40C)</t>
+  </si>
+  <si>
+    <t>For the production sourdough (fermenting for 12-18 hours):</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>rye sourdough starter</t>
+  </si>
+  <si>
+    <t>For the main dough:</t>
+  </si>
+  <si>
+    <t>production sourdough (the rest can be used for another loaf, or binned)</t>
+  </si>
+  <si>
+    <t>rye flour (light or dark)</t>
+  </si>
+  <si>
+    <t>sea salt</t>
+  </si>
+  <si>
+    <t>coarsely ground coriander plus a little extra to sprinkle on top of the loaf</t>
+  </si>
+  <si>
+    <t>molasses</t>
+  </si>
+  <si>
+    <t> barley malt extract</t>
+  </si>
+  <si>
+    <t>warm water (at 35C)</t>
+  </si>
+  <si>
+    <t>whole coriander seeds, to sprinkle in the tin</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>On day 1 mix 25g dark rye flour with 50g very warm water in a large jar or a plastic tub with a lid. Keep it in the warmest place in the house you can find (airing cupboard does well). On day 2, 3 and 4 add another 25g of rye flour and 50g of warm water. You should get a bubbly starter – bubbles are the sign of life here, it doesn’t significantly expand. Let the starter ferment for 24 hours after the last feeding before making the production sourdough.</t>
+  </si>
+  <si>
+    <t>Mix 50g of the starter with the other ingredients for production sourdough. The rest of the starter can be stored in the fridge, and fed with 25g flour and 50g water 24 hours ahead of your next rye loaf.</t>
+  </si>
+  <si>
+    <t>The production sourdough needs to prove in a warm place for 12-18 hours.</t>
+  </si>
+  <si>
+    <t>Prepare a small loaf tin by greasing it thoroughly with butter. Sprinkle some whole coriander seeds over the bottom of the tin.</t>
+  </si>
+  <si>
+    <t>To make the Borodinsky dough, mix all the ingredients to a soft dough – it won’t be anything like wheat dough, not stretchy or elastic, rather resembling a brownish concrete mix or mud! Turn it out onto wet worktop, wet your hands too and form a rough shape of a loaf. Place it in the tin, cover with cling film and leave in a warm place for up to 6 hours. If you use just dark flour for the main loaf, the rise will be very slow indeed – but the flavour more intense.</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>temperature unit</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>10% edmonds wholemeal n </t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>10% freshly "pounded" nz pearl barley sourdough</t>
+  </si>
+  <si>
+    <t>At 75% hydration</t>
+  </si>
+  <si>
+    <t>20% liquidstarter used.</t>
+  </si>
+  <si>
+    <t>Added chopped dates.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,6 +468,37 @@
       <color rgb="FF444444"/>
       <name val="Lato"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1D2129"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF1D2129"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -397,7 +517,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -451,8 +571,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,9 +582,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -489,6 +619,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -515,6 +646,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -847,7 +979,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
@@ -1325,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1733,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
@@ -1751,10 +1883,11 @@
     <col min="10" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="84">
+    <row r="1" spans="1:15" ht="84">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -1797,8 +1930,11 @@
       <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1814,8 +1950,11 @@
       <c r="E2" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="4" t="s">
         <v>63</v>
       </c>
@@ -1826,7 +1965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="C4" s="4" t="s">
         <v>64</v>
       </c>
@@ -1837,7 +1976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1848,7 +1987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
@@ -1862,12 +2001,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="C7" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
@@ -1878,7 +2017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="C9" s="4" t="s">
         <v>72</v>
       </c>
@@ -1889,7 +2028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="C10" s="4" t="s">
         <v>73</v>
       </c>
@@ -1900,7 +2039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="C11" s="4" t="s">
         <v>74</v>
       </c>
@@ -1911,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="C12" s="4" t="s">
         <v>76</v>
       </c>
@@ -1922,7 +2061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
@@ -1930,7 +2069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="C14" s="4" t="s">
         <v>69</v>
       </c>
@@ -1938,7 +2077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="C15" s="4" t="s">
         <v>75</v>
       </c>
@@ -1949,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="C16" s="4" t="s">
         <v>77</v>
       </c>
@@ -1957,6 +2096,594 @@
     <row r="17" spans="3:3">
       <c r="C17" s="4" t="s">
         <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="1">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1">
+        <f>B3/3</f>
+        <v>66.666666666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1">
+        <v>200</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F21" si="0">B4/3</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="J4" s="1">
+        <v>75</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1">
+        <v>220</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>110</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="J9" s="1">
+        <v>80</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1">
+        <v>220</v>
+      </c>
+      <c r="E10" s="1">
+        <v>110</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>73.333333333333329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>500</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>333.33333333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="1">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1">
+        <v>120</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="E15" s="1">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1">
+        <v>500</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>250</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1">
+        <v>240</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="E18" s="1">
+        <v>120</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="1">
+        <v>300</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>150</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1">
+        <v>400</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>200</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="1">
+        <v>450</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="E21" s="1">
+        <v>225</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="128.83203125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="1">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="1">
+        <v>150</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="1">
+        <v>300</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="1">
+        <v>270</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1">
+        <v>230</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1969,391 +2696,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>3</v>
-      </c>
-      <c r="I1">
-        <v>6</v>
-      </c>
-      <c r="J1">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5">
-        <v>200</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <f>B5/3</f>
-        <v>66.666666666666671</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6">
-        <v>200</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F23" si="0">B6/3</f>
-        <v>66.666666666666671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <v>220</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>110</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>73.333333333333329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12">
-        <v>220</v>
-      </c>
-      <c r="E12">
-        <v>110</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>73.333333333333329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>500</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>333.33333333333331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17">
-        <v>120</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="E17">
-        <v>60</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19">
-        <v>500</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E19">
-        <v>250</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>166.66666666666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20">
-        <v>240</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.24</v>
-      </c>
-      <c r="E20">
-        <v>120</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21">
-        <v>300</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E21">
-        <v>150</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22">
-        <v>400</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E22">
-        <v>200</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23">
-        <v>450</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="E23">
-        <v>225</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25">
-        <f>SUM(B15:B23)</f>
-        <v>3045</v>
-      </c>
-      <c r="E25">
-        <f>SUM(E15:E23)</f>
-        <v>1523</v>
-      </c>
-      <c r="F25">
-        <f>SUM(F15:F24)</f>
-        <v>1015</v>
+      <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="12" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>